<commit_message>
perbaikan final untuk app
</commit_message>
<xml_diff>
--- a/uploads/formatImport/data_meterpelanggan.xlsx
+++ b/uploads/formatImport/data_meterpelanggan.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rtiadi\Desktop\pengaduan-pdam\public\uploads\formatImport\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\pengaduan-pdam\uploads\formatImport\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{887060DD-D474-4C6C-BB57-4E9D17469503}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E9BFBAE-3018-4BE4-A953-C231729B701D}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4620" yWindow="3045" windowWidth="15375" windowHeight="7875" xr2:uid="{F6E9E287-5DF2-4BB8-BF99-39A5488DEF69}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{F6E9E287-5DF2-4BB8-BF99-39A5488DEF69}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="7">
   <si>
     <t>no_sambung</t>
   </si>
@@ -38,22 +38,25 @@
     <t>0002</t>
   </si>
   <si>
-    <t>tanggal_meter</t>
-  </si>
-  <si>
     <t>meter</t>
   </si>
   <si>
     <t>0001</t>
+  </si>
+  <si>
+    <t>bulan_meter</t>
+  </si>
+  <si>
+    <t>tahun_meter</t>
+  </si>
+  <si>
+    <t>Agustus</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd;@"/>
-  </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -92,7 +95,7 @@
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -407,55 +410,64 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{14B9A1E8-4137-4C04-B3B2-9E9D281EA695}">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="B1" t="s">
+      <c r="D1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="2">
+        <v>2020</v>
+      </c>
+      <c r="C2">
+        <v>100000</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C1" t="s">
-        <v>0</v>
-      </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="2">
-        <v>44054</v>
-      </c>
-      <c r="B2">
-        <v>100000</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="2">
-        <v>44055</v>
-      </c>
-      <c r="B3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="2">
+        <v>2020</v>
+      </c>
+      <c r="C3">
         <v>150000</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="D3" s="1" t="s">
         <v>1</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>